<commit_message>
Continued base study and work on excel only
</commit_message>
<xml_diff>
--- a/4_Applied ML with Python/Practice/Lines_Excel_Linear Regression.xlsx
+++ b/4_Applied ML with Python/Practice/Lines_Excel_Linear Regression.xlsx
@@ -8,14 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repos\CourseraPlus\4_Applied ML with Python\Practice\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B31C609B-37E3-426D-8BB8-B24A1B56804D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAE97C93-18F6-472C-B4FD-A1A0D2076F35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{995899B7-4EAD-4DF0-B805-458A0F3CCA07}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{995899B7-4EAD-4DF0-B805-458A0F3CCA07}"/>
   </bookViews>
   <sheets>
-    <sheet name="Main" sheetId="1" r:id="rId1"/>
-    <sheet name="Reference" sheetId="2" r:id="rId2"/>
+    <sheet name="Simple" sheetId="1" r:id="rId1"/>
+    <sheet name="Bill &amp; Tips" sheetId="3" r:id="rId2"/>
+    <sheet name="Reference" sheetId="2" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="xmean">'Bill &amp; Tips'!$C$11</definedName>
+    <definedName name="ymean">'Bill &amp; Tips'!$D$11</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -36,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
   <si>
     <t>Graph Values</t>
   </si>
@@ -79,17 +84,70 @@
   <si>
     <t>Plot</t>
   </si>
+  <si>
+    <t>Meal</t>
+  </si>
+  <si>
+    <t>Bill</t>
+  </si>
+  <si>
+    <t>Tips</t>
+  </si>
+  <si>
+    <t>Bill Deviation</t>
+  </si>
+  <si>
+    <t>Bills and Tips Regression</t>
+  </si>
+  <si>
+    <t>Tips Deviation</t>
+  </si>
+  <si>
+    <t>Deviation Products</t>
+  </si>
+  <si>
+    <t>Bill Deviations Squared</t>
+  </si>
+  <si>
+    <t>(product)</t>
+  </si>
+  <si>
+    <t>(xi - xmean)^2</t>
+  </si>
+  <si>
+    <t>(x)</t>
+  </si>
+  <si>
+    <t>(y)</t>
+  </si>
+  <si>
+    <t>(xi - xmean)</t>
+  </si>
+  <si>
+    <t>(yi - ymean)</t>
+  </si>
+  <si>
+    <t>Mean</t>
+  </si>
+  <si>
+    <t>Sum -&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">b0 = </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="5">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="170" formatCode="0.000000"/>
-    <numFmt numFmtId="171" formatCode="0.0000000"/>
+    <numFmt numFmtId="164" formatCode="0.000000"/>
+    <numFmt numFmtId="165" formatCode="0.0000000"/>
+    <numFmt numFmtId="167" formatCode="_-* #,##0.0000_-;\-* #,##0.0000_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="168" formatCode="_-* #,##0.00000_-;\-* #,##0.00000_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -148,8 +206,22 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -162,8 +234,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor theme="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -171,12 +255,67 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -192,13 +331,52 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="170" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="171" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="43" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="2" fillId="4" borderId="0" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="2" fillId="4" borderId="0" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -207,6 +385,9 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="5">
+    <dxf>
+      <numFmt numFmtId="35" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -224,9 +405,6 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="35" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="35" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     </dxf>
     <dxf>
@@ -436,7 +614,7 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>Main!$C$4:$C$10</c:f>
+              <c:f>Simple!$C$4:$C$10</c:f>
               <c:numCache>
                 <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="7"/>
@@ -549,7 +727,7 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>Main!$D$4:$D$10</c:f>
+              <c:f>Simple!$D$4:$D$10</c:f>
               <c:numCache>
                 <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="7"/>
@@ -581,6 +759,634 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000005-9291-4ED9-9CA8-2F17280C6A04}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="t"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="95806880"/>
+        <c:axId val="95793152"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="95806880"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>X-Values</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="dk1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="95793152"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="95793152"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                  <a:alpha val="54000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Y-Values</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="95806880"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:dTable>
+        <c:showHorzBorder val="1"/>
+        <c:showVertBorder val="1"/>
+        <c:showOutline val="1"/>
+        <c:showKeys val="1"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="dk1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr rtl="0">
+              <a:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+      </c:dTable>
+      <c:spPr>
+        <a:pattFill prst="ltDnDiag">
+          <a:fgClr>
+            <a:schemeClr val="dk1">
+              <a:lumMod val="15000"/>
+              <a:lumOff val="85000"/>
+            </a:schemeClr>
+          </a:fgClr>
+          <a:bgClr>
+            <a:schemeClr val="lt1"/>
+          </a:bgClr>
+        </a:pattFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="lt1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="50000"/>
+                    <a:lumOff val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mj-lt"/>
+                <a:ea typeface="+mj-ea"/>
+                <a:cs typeface="+mj-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>y-plot</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> with generalized line</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mj-lt"/>
+              <a:ea typeface="+mj-ea"/>
+              <a:cs typeface="+mj-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="dk1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>'Bill &amp; Tips'!$C$5:$C$10</c:f>
+              <c:numCache>
+                <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>108</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>88</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>99</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>51</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-5F81-45FB-A381-F9167411D0BE}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Trendline</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="t"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="dk1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>'Bill &amp; Tips'!$D$5:$D$10</c:f>
+              <c:numCache>
+                <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-5F81-45FB-A381-F9167411D0BE}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -953,7 +1759,595 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="12">
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="232">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="22225" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="15875">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="800" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="ltDnDiag">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+            <a:alpha val="51000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="ltDnDiag">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
+    </cs:spPr>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="major">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="ltDnDiag">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="232">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -1546,6 +2940,110 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>4761</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>114299</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>123824</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{535730AD-4C82-4CC5-8C12-E356F4591565}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ADED61B2-CC9E-4257-9DF9-03C1D76A0C9B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="142875" y="2743200"/>
+          <a:ext cx="2266950" cy="542925"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -1606,10 +3104,10 @@
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{D80E1A59-FE2D-40B7-A59B-EE0E5FE42168}" name="X" dataDxfId="3"/>
     <tableColumn id="2" xr3:uid="{B098714D-CC10-45C2-8D75-C301525DF26E}" name="y" dataDxfId="2" dataCellStyle="Comma"/>
-    <tableColumn id="6" xr3:uid="{184FA016-1ED8-4EDB-A016-757562BC1DA5}" name="Plot" dataDxfId="0" dataCellStyle="Comma">
+    <tableColumn id="6" xr3:uid="{184FA016-1ED8-4EDB-A016-757562BC1DA5}" name="Plot" dataDxfId="1" dataCellStyle="Comma">
       <calculatedColumnFormula>$F$15*Table1[[#This Row],[X]]+$C$15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{334D0BF8-E99F-4951-9277-978C765A67B2}" name="X.y" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{334D0BF8-E99F-4951-9277-978C765A67B2}" name="X.y" dataDxfId="0"/>
     <tableColumn id="4" xr3:uid="{04DCFAC7-F8AC-4F98-A3B8-1467EC661F31}" name="X^2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1915,7 +3413,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B52F56F-293C-43B2-9C80-EEC3C02E9B0E}">
   <dimension ref="A2:F18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="R10" sqref="R10"/>
     </sheetView>
   </sheetViews>
@@ -1962,7 +3460,7 @@
         <v>1.5</v>
       </c>
       <c r="F4" s="2">
-        <f>B4*B4</f>
+        <f t="shared" ref="F4:F10" si="0">B4*B4</f>
         <v>1</v>
       </c>
     </row>
@@ -1978,11 +3476,11 @@
         <v>4.0571428571428543</v>
       </c>
       <c r="E5" s="4">
-        <f t="shared" ref="E5:E10" si="0">B5*C5</f>
+        <f t="shared" ref="E5:E10" si="1">B5*C5</f>
         <v>6.6</v>
       </c>
       <c r="F5" s="2">
-        <f>B5*B5</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
     </row>
@@ -1998,11 +3496,11 @@
         <v>6.1999999999999984</v>
       </c>
       <c r="E6" s="4">
+        <f t="shared" si="1"/>
+        <v>19.5</v>
+      </c>
+      <c r="F6" s="2">
         <f t="shared" si="0"/>
-        <v>19.5</v>
-      </c>
-      <c r="F6" s="2">
-        <f>B6*B6</f>
         <v>9</v>
       </c>
     </row>
@@ -2018,11 +3516,11 @@
         <v>8.3428571428571416</v>
       </c>
       <c r="E7" s="4">
+        <f t="shared" si="1"/>
+        <v>38</v>
+      </c>
+      <c r="F7" s="2">
         <f t="shared" si="0"/>
-        <v>38</v>
-      </c>
-      <c r="F7" s="2">
-        <f>B7*B7</f>
         <v>16</v>
       </c>
     </row>
@@ -2038,11 +3536,11 @@
         <v>10.485714285714286</v>
       </c>
       <c r="E8" s="4">
+        <f t="shared" si="1"/>
+        <v>58</v>
+      </c>
+      <c r="F8" s="2">
         <f t="shared" si="0"/>
-        <v>58</v>
-      </c>
-      <c r="F8" s="2">
-        <f>B8*B8</f>
         <v>25</v>
       </c>
     </row>
@@ -2058,11 +3556,11 @@
         <v>12.62857142857143</v>
       </c>
       <c r="E9" s="4">
+        <f t="shared" si="1"/>
+        <v>72</v>
+      </c>
+      <c r="F9" s="2">
         <f t="shared" si="0"/>
-        <v>72</v>
-      </c>
-      <c r="F9" s="2">
-        <f>B9*B9</f>
         <v>36</v>
       </c>
     </row>
@@ -2078,11 +3576,11 @@
         <v>14.771428571428574</v>
       </c>
       <c r="E10" s="4">
+        <f t="shared" si="1"/>
+        <v>98</v>
+      </c>
+      <c r="F10" s="2">
         <f t="shared" si="0"/>
-        <v>98</v>
-      </c>
-      <c r="F10" s="2">
-        <f>B10*B10</f>
         <v>49</v>
       </c>
     </row>
@@ -2091,11 +3589,11 @@
         <v>5</v>
       </c>
       <c r="B11" s="1">
-        <f t="shared" ref="B11:F11" si="1">SUM(B4:B10)</f>
+        <f t="shared" ref="B11:F11" si="2">SUM(B4:B10)</f>
         <v>28</v>
       </c>
       <c r="C11" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>58.4</v>
       </c>
       <c r="D11" s="15">
@@ -2103,11 +3601,11 @@
         <v>59.771428571428601</v>
       </c>
       <c r="E11" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>293.60000000000002</v>
       </c>
       <c r="F11" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>140</v>
       </c>
     </row>
@@ -2167,6 +3665,308 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB946D3E-1162-4E03-884C-51FAE36A8CB7}">
+  <dimension ref="A2:I18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="1.875" customWidth="1"/>
+    <col min="5" max="5" width="13.75" customWidth="1"/>
+    <col min="6" max="7" width="16" customWidth="1"/>
+    <col min="8" max="8" width="17.375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:9" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="B2" s="22" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" s="23" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+      <c r="B3" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3" s="26" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" s="23" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="B4" s="24"/>
+      <c r="C4" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="G4" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="H4" s="25" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B5" s="16">
+        <v>1</v>
+      </c>
+      <c r="C5" s="17">
+        <v>34</v>
+      </c>
+      <c r="D5" s="17">
+        <v>5</v>
+      </c>
+      <c r="E5" s="18">
+        <f t="shared" ref="E5:E10" si="0">C5-xmean</f>
+        <v>-40</v>
+      </c>
+      <c r="F5" s="18">
+        <f t="shared" ref="F5:F10" si="1">D5-ymean</f>
+        <v>-5</v>
+      </c>
+      <c r="G5" s="18">
+        <f>E5*F5</f>
+        <v>200</v>
+      </c>
+      <c r="H5" s="27">
+        <f>E5^2</f>
+        <v>1600</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B6" s="16">
+        <v>2</v>
+      </c>
+      <c r="C6" s="17">
+        <v>108</v>
+      </c>
+      <c r="D6" s="17">
+        <v>17</v>
+      </c>
+      <c r="E6" s="18">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
+      <c r="F6" s="18">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="G6" s="18">
+        <f t="shared" ref="G6:G10" si="2">E6*F6</f>
+        <v>238</v>
+      </c>
+      <c r="H6" s="27">
+        <f t="shared" ref="H6:H10" si="3">E6^2</f>
+        <v>1156</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B7" s="16">
+        <v>3</v>
+      </c>
+      <c r="C7" s="17">
+        <v>64</v>
+      </c>
+      <c r="D7" s="17">
+        <v>11</v>
+      </c>
+      <c r="E7" s="18">
+        <f t="shared" si="0"/>
+        <v>-10</v>
+      </c>
+      <c r="F7" s="18">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="G7" s="18">
+        <f t="shared" si="2"/>
+        <v>-10</v>
+      </c>
+      <c r="H7" s="27">
+        <f t="shared" si="3"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B8" s="16">
+        <v>4</v>
+      </c>
+      <c r="C8" s="17">
+        <v>88</v>
+      </c>
+      <c r="D8" s="17">
+        <v>8</v>
+      </c>
+      <c r="E8" s="18">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="F8" s="18">
+        <f t="shared" si="1"/>
+        <v>-2</v>
+      </c>
+      <c r="G8" s="18">
+        <f t="shared" si="2"/>
+        <v>-28</v>
+      </c>
+      <c r="H8" s="27">
+        <f t="shared" si="3"/>
+        <v>196</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B9" s="16">
+        <v>5</v>
+      </c>
+      <c r="C9" s="17">
+        <v>99</v>
+      </c>
+      <c r="D9" s="17">
+        <v>14</v>
+      </c>
+      <c r="E9" s="18">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="F9" s="18">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="G9" s="18">
+        <f t="shared" si="2"/>
+        <v>100</v>
+      </c>
+      <c r="H9" s="27">
+        <f t="shared" si="3"/>
+        <v>625</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B10" s="16">
+        <v>6</v>
+      </c>
+      <c r="C10" s="17">
+        <v>51</v>
+      </c>
+      <c r="D10" s="17">
+        <v>5</v>
+      </c>
+      <c r="E10" s="18">
+        <f t="shared" si="0"/>
+        <v>-23</v>
+      </c>
+      <c r="F10" s="18">
+        <f t="shared" si="1"/>
+        <v>-5</v>
+      </c>
+      <c r="G10" s="18">
+        <f t="shared" si="2"/>
+        <v>115</v>
+      </c>
+      <c r="H10" s="27">
+        <f t="shared" si="3"/>
+        <v>529</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A11" s="5"/>
+      <c r="B11" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" s="21">
+        <f>AVERAGE(C5:C10)</f>
+        <v>74</v>
+      </c>
+      <c r="D11" s="21">
+        <f>AVERAGE(D5:D10)</f>
+        <v>10</v>
+      </c>
+      <c r="E11" s="20"/>
+      <c r="F11" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="G11" s="21">
+        <f>SUM(G5:G10)</f>
+        <v>615</v>
+      </c>
+      <c r="H11" s="21">
+        <f>SUM(H5:H10)</f>
+        <v>4206</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="B13" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" s="29">
+        <f>G11/H11</f>
+        <v>0.14621968616262482</v>
+      </c>
+      <c r="D13" s="7"/>
+      <c r="E13" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="F13" s="30">
+        <f>ymean-C13*xmean</f>
+        <v>-0.82025677603423652</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="B15" s="1"/>
+      <c r="C15"/>
+      <c r="D15"/>
+      <c r="E15"/>
+      <c r="F15"/>
+      <c r="G15"/>
+      <c r="H15"/>
+      <c r="I15"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="8"/>
+    </row>
+    <row r="18" spans="2:8" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B18" s="13"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="12"/>
+      <c r="F18" s="12"/>
+      <c r="G18" s="12"/>
+      <c r="H18" s="11"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{444B31FE-9D94-4105-9694-D16CEE94268F}">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>

<commit_message>
Regression studies - SST SSE and SSR
</commit_message>
<xml_diff>
--- a/4_Applied ML with Python/Practice/Lines_Excel_Linear Regression.xlsx
+++ b/4_Applied ML with Python/Practice/Lines_Excel_Linear Regression.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repos\CourseraPlus\4_Applied ML with Python\Practice\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAE97C93-18F6-472C-B4FD-A1A0D2076F35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FC9AE8C-11B7-4415-8609-09B6F1668336}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{995899B7-4EAD-4DF0-B805-458A0F3CCA07}"/>
   </bookViews>
@@ -18,6 +18,8 @@
     <sheet name="Reference" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
+    <definedName name="b">'Bill &amp; Tips'!$C$13</definedName>
+    <definedName name="b0">'Bill &amp; Tips'!$F$13</definedName>
     <definedName name="xmean">'Bill &amp; Tips'!$C$11</definedName>
     <definedName name="ymean">'Bill &amp; Tips'!$D$11</definedName>
   </definedNames>
@@ -41,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="38">
   <si>
     <t>Graph Values</t>
   </si>
@@ -106,25 +108,13 @@
     <t>Deviation Products</t>
   </si>
   <si>
-    <t>Bill Deviations Squared</t>
-  </si>
-  <si>
     <t>(product)</t>
-  </si>
-  <si>
-    <t>(xi - xmean)^2</t>
   </si>
   <si>
     <t>(x)</t>
   </si>
   <si>
     <t>(y)</t>
-  </si>
-  <si>
-    <t>(xi - xmean)</t>
-  </si>
-  <si>
-    <t>(yi - ymean)</t>
   </si>
   <si>
     <t>Mean</t>
@@ -135,6 +125,39 @@
   <si>
     <t xml:space="preserve">b0 = </t>
   </si>
+  <si>
+    <t>Error</t>
+  </si>
+  <si>
+    <t>y - yi</t>
+  </si>
+  <si>
+    <t>Squared Error</t>
+  </si>
+  <si>
+    <t>(y - yi)^2</t>
+  </si>
+  <si>
+    <t>Predicted Amount</t>
+  </si>
+  <si>
+    <t>(y - ymean)</t>
+  </si>
+  <si>
+    <t>(x - xmean)</t>
+  </si>
+  <si>
+    <t>(x - xmean)^2</t>
+  </si>
+  <si>
+    <t>yi = b * x + b0</t>
+  </si>
+  <si>
+    <t>SSE -&gt;</t>
+  </si>
+  <si>
+    <t>Deviations Squared</t>
+  </si>
 </sst>
 </file>
 
@@ -144,10 +167,10 @@
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="0.000000"/>
     <numFmt numFmtId="165" formatCode="0.0000000"/>
-    <numFmt numFmtId="167" formatCode="_-* #,##0.0000_-;\-* #,##0.0000_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="168" formatCode="_-* #,##0.00000_-;\-* #,##0.00000_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="166" formatCode="_-* #,##0.0000_-;\-* #,##0.0000_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="167" formatCode="_-* #,##0.00000_-;\-* #,##0.00000_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -217,6 +240,12 @@
       <b/>
       <sz val="15"/>
       <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFC00000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -315,7 +344,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -373,10 +402,19 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="166" fontId="2" fillId="4" borderId="0" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="167" fontId="2" fillId="4" borderId="0" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="2" fillId="4" borderId="0" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="11" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="2" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1115,27 +1153,26 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
+              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="dk1">
-                    <a:lumMod val="50000"/>
-                    <a:lumOff val="50000"/>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mj-lt"/>
-                <a:ea typeface="+mj-ea"/>
-                <a:cs typeface="+mj-cs"/>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>y-plot</a:t>
+              <a:rPr lang="en-GB"/>
+              <a:t>Tips</a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> with generalized line</a:t>
+              <a:rPr lang="en-GB" baseline="0"/>
+              <a:t> vs Pred. Tips</a:t>
             </a:r>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-GB"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -1152,16 +1189,15 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
+            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="dk1">
-                  <a:lumMod val="50000"/>
-                  <a:lumOff val="50000"/>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="85000"/>
                 </a:schemeClr>
               </a:solidFill>
-              <a:latin typeface="+mj-lt"/>
-              <a:ea typeface="+mj-ea"/>
-              <a:cs typeface="+mj-cs"/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
           <a:endParaRPr lang="en-US"/>
@@ -1177,185 +1213,27 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:v>Tips</c:v>
+          </c:tx>
           <c:spPr>
             <a:ln w="22225" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent2"/>
+                <a:srgbClr val="00B050"/>
               </a:solidFill>
-              <a:round/>
             </a:ln>
-            <a:effectLst/>
+            <a:effectLst>
+              <a:glow rad="139700">
+                <a:schemeClr val="accent2">
+                  <a:satMod val="175000"/>
+                  <a:alpha val="14000"/>
+                </a:schemeClr>
+              </a:glow>
+            </a:effectLst>
           </c:spPr>
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
-          <c:dLbls>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="dk1">
-                        <a:lumMod val="75000"/>
-                        <a:lumOff val="25000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="en-US"/>
-              </a:p>
-            </c:txPr>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="1"/>
-                <c15:leaderLines>
-                  <c:spPr>
-                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                      <a:solidFill>
-                        <a:schemeClr val="dk1">
-                          <a:lumMod val="35000"/>
-                          <a:lumOff val="65000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:round/>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c15:leaderLines>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
-          <c:val>
-            <c:numRef>
-              <c:f>'Bill &amp; Tips'!$C$5:$C$10</c:f>
-              <c:numCache>
-                <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>34</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>108</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>64</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>88</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>99</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>51</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-5F81-45FB-A381-F9167411D0BE}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:v>Trendline</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="22225" cap="rnd">
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:dLbls>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="dk1">
-                        <a:lumMod val="75000"/>
-                        <a:lumOff val="25000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="en-US"/>
-              </a:p>
-            </c:txPr>
-            <c:dLblPos val="t"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="1"/>
-                <c15:leaderLines>
-                  <c:spPr>
-                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                      <a:solidFill>
-                        <a:schemeClr val="dk1">
-                          <a:lumMod val="35000"/>
-                          <a:lumOff val="65000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:round/>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c15:leaderLines>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
           <c:val>
             <c:numRef>
               <c:f>'Bill &amp; Tips'!$D$5:$D$10</c:f>
@@ -1386,19 +1264,116 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-5F81-45FB-A381-F9167411D0BE}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Pred. Tips</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="FFFF00"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst>
+              <a:glow rad="139700">
+                <a:schemeClr val="accent4">
+                  <a:satMod val="175000"/>
+                  <a:alpha val="14000"/>
+                </a:schemeClr>
+              </a:glow>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Bill &amp; Tips'!$I$5:$I$10</c:f>
+              <c:numCache>
+                <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>4.1512125534950073</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>14.971469329529244</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.5378031383737518</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12.047075606276747</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>13.655492154065621</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.6369472182596292</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-5F81-45FB-A381-F9167411D0BE}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="t"/>
           <c:showLegendKey val="0"/>
-          <c:showVal val="1"/>
+          <c:showVal val="0"/>
           <c:showCatName val="0"/>
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:upDownBars>
+          <c:gapWidth val="315"/>
+          <c:upBars>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:upBars>
+          <c:downBars>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:downBars>
+        </c:upDownBars>
         <c:smooth val="0"/>
         <c:axId val="95806880"/>
         <c:axId val="95793152"/>
@@ -1410,6 +1385,31 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:gradFill>
+                <a:gsLst>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="0">
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
         <c:title>
           <c:tx>
             <c:rich>
@@ -1419,9 +1419,8 @@
                 <a:pPr>
                   <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="dk1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="75000"/>
                       </a:schemeClr>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
@@ -1431,7 +1430,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-GB"/>
-                  <a:t>X-Values</a:t>
+                  <a:t>Meals</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -1451,9 +1450,8 @@
               <a:pPr>
                 <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
-                    <a:schemeClr val="dk1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="75000"/>
                     </a:schemeClr>
                   </a:solidFill>
                   <a:latin typeface="+mn-lt"/>
@@ -1466,19 +1464,13 @@
           </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
+        <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="dk1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
+          <a:ln>
+            <a:noFill/>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -1487,11 +1479,10 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="dk1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -1519,13 +1510,23 @@
         <c:majorGridlines>
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="dk1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                  <a:alpha val="54000"/>
-                </a:schemeClr>
-              </a:solidFill>
+              <a:gradFill>
+                <a:gsLst>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="0">
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -1540,9 +1541,8 @@
                 <a:pPr>
                   <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="dk1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="75000"/>
                       </a:schemeClr>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
@@ -1552,7 +1552,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-GB"/>
-                  <a:t>Y-Values</a:t>
+                  <a:t>Tips</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -1572,9 +1572,8 @@
               <a:pPr>
                 <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
-                    <a:schemeClr val="dk1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="75000"/>
                     </a:schemeClr>
                   </a:solidFill>
                   <a:latin typeface="+mn-lt"/>
@@ -1587,7 +1586,7 @@
           </c:txPr>
         </c:title>
         <c:numFmt formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
+        <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
@@ -1604,9 +1603,8 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="dk1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -1628,14 +1626,13 @@
         <c:showKeys val="1"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:ln w="9525">
             <a:solidFill>
               <a:schemeClr val="dk1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
+                <a:lumMod val="50000"/>
+                <a:lumOff val="50000"/>
               </a:schemeClr>
             </a:solidFill>
-            <a:round/>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -1644,11 +1641,10 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr rtl="0">
-              <a:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="dk1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -1661,17 +1657,7 @@
         </c:txPr>
       </c:dTable>
       <c:spPr>
-        <a:pattFill prst="ltDnDiag">
-          <a:fgClr>
-            <a:schemeClr val="dk1">
-              <a:lumMod val="15000"/>
-              <a:lumOff val="85000"/>
-            </a:schemeClr>
-          </a:fgClr>
-          <a:bgClr>
-            <a:schemeClr val="lt1"/>
-          </a:bgClr>
-        </a:pattFill>
+        <a:noFill/>
         <a:ln>
           <a:noFill/>
         </a:ln>
@@ -1691,7 +1677,10 @@
   </c:chart>
   <c:spPr>
     <a:solidFill>
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
       <a:solidFill>
@@ -2348,15 +2337,14 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="232">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="236">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" b="1" kern="1200"/>
@@ -2366,23 +2354,11 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:categoryAxis>
   <cs:chartArea>
     <cs:lnRef idx="0"/>
@@ -2393,7 +2369,10 @@
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
-        <a:schemeClr val="lt1"/>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
       </a:solidFill>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
@@ -2412,9 +2391,8 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
+      <a:schemeClr val="lt1">
         <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -2424,23 +2402,18 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="15000"/>
+        <a:lumOff val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
-        <a:schemeClr val="lt1"/>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
       </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
     <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
@@ -2448,41 +2421,73 @@
     </cs:bodyPr>
   </cs:dataLabelCallout>
   <cs:dataPoint>
-    <cs:lnRef idx="0"/>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
     <cs:fillRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0"/>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
     <cs:fontRef idx="minor">
       <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
     </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
     <cs:fontRef idx="minor">
       <a:schemeClr val="dk1"/>
     </cs:fontRef>
@@ -2491,8 +2496,15 @@
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:round/>
       </a:ln>
+      <a:effectLst>
+        <a:glow rad="139700">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="14000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
     </cs:spPr>
   </cs:dataPointLine>
   <cs:dataPointMarker>
@@ -2502,23 +2514,30 @@
     <cs:fillRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0"/>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
     <cs:fontRef idx="minor">
       <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
-        <a:schemeClr val="lt1"/>
+        <a:schemeClr val="phClr">
+          <a:lumMod val="60000"/>
+          <a:lumOff val="40000"/>
+        </a:schemeClr>
       </a:solidFill>
-      <a:ln w="15875">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
     </cs:spPr>
   </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointMarkerLayout symbol="circle" size="4"/>
   <cs:dataPointWireframe>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
@@ -2542,43 +2561,40 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="800" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="dk1">
             <a:lumMod val="50000"/>
             <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="50000"/>
+          <a:lumOff val="50000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="75000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -2593,11 +2609,10 @@
       <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -2612,11 +2627,10 @@
       <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="dk1">
+          <a:schemeClr val="lt1">
             <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -2630,19 +2644,6 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="dk1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:pattFill prst="ltDnDiag">
-        <a:fgClr>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:fgClr>
-        <a:bgClr>
-          <a:schemeClr val="lt1"/>
-        </a:bgClr>
-      </a:pattFill>
-    </cs:spPr>
   </cs:floor>
   <cs:gridlineMajor>
     <cs:lnRef idx="0"/>
@@ -2653,13 +2654,23 @@
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-            <a:alpha val="54000"/>
-          </a:schemeClr>
-        </a:solidFill>
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="100000">
+              <a:schemeClr val="dk1">
+                <a:lumMod val="75000"/>
+                <a:lumOff val="25000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="0">
+              <a:schemeClr val="dk1">
+                <a:lumMod val="65000"/>
+                <a:lumOff val="35000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
         <a:round/>
       </a:ln>
     </cs:spPr>
@@ -2673,13 +2684,25 @@
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-            <a:alpha val="51000"/>
-          </a:schemeClr>
-        </a:solidFill>
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="100000">
+              <a:schemeClr val="dk1">
+                <a:lumMod val="75000"/>
+                <a:lumOff val="25000"/>
+                <a:alpha val="25000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="0">
+              <a:schemeClr val="dk1">
+                <a:lumMod val="65000"/>
+                <a:lumOff val="35000"/>
+                <a:alpha val="25000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
         <a:round/>
       </a:ln>
     </cs:spPr>
@@ -2692,11 +2715,10 @@
       <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -2711,11 +2733,10 @@
       <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -2727,9 +2748,8 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -2741,19 +2761,6 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="dk1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:pattFill prst="ltDnDiag">
-        <a:fgClr>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:fgClr>
-        <a:bgClr>
-          <a:schemeClr val="lt1"/>
-        </a:bgClr>
-      </a:pattFill>
-    </cs:spPr>
   </cs:plotArea>
   <cs:plotArea3D>
     <cs:lnRef idx="0"/>
@@ -2762,20 +2769,14 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="dk1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-    </cs:spPr>
   </cs:plotArea3D>
   <cs:seriesAxis>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -2788,11 +2789,10 @@
       <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -2803,13 +2803,12 @@
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
-    <cs:fontRef idx="major">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="50000"/>
-        <a:lumOff val="50000"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1600" b="1" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0"/>
+    <cs:defRPr sz="1400" b="1" kern="1200" cap="none" baseline="0"/>
   </cs:title>
   <cs:trendline>
     <cs:lnRef idx="0">
@@ -2818,12 +2817,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="19050" cap="rnd">
+      <a:ln w="25400" cap="rnd">
         <a:solidFill>
-          <a:schemeClr val="phClr"/>
+          <a:schemeClr val="phClr">
+            <a:alpha val="50000"/>
+          </a:schemeClr>
         </a:solidFill>
       </a:ln>
     </cs:spPr>
@@ -2833,9 +2834,8 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -2849,13 +2849,14 @@
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
-        <a:schemeClr val="lt1"/>
+        <a:schemeClr val="lt1">
+          <a:lumMod val="85000"/>
+        </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="dk1">
             <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -2867,9 +2868,8 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -2881,19 +2881,6 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="dk1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:pattFill prst="ltDnDiag">
-        <a:fgClr>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:fgClr>
-        <a:bgClr>
-          <a:schemeClr val="lt1"/>
-        </a:bgClr>
-      </a:pattFill>
-    </cs:spPr>
   </cs:wall>
 </cs:chartStyle>
 </file>
@@ -2943,16 +2930,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>4761</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>114299</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>223836</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>200025</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>123824</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>1028700</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2988,7 +2975,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
+      <xdr:colOff>666750</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>85725</xdr:rowOff>
     </xdr:to>
@@ -3666,26 +3653,34 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB946D3E-1162-4E03-884C-51FAE36A8CB7}">
-  <dimension ref="A2:I18"/>
+  <dimension ref="A1:K18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="1.875" customWidth="1"/>
-    <col min="5" max="5" width="13.75" customWidth="1"/>
-    <col min="6" max="7" width="16" customWidth="1"/>
-    <col min="8" max="8" width="17.375" customWidth="1"/>
+    <col min="2" max="2" width="6.75" customWidth="1"/>
+    <col min="3" max="3" width="7.625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.75" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.75" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" ht="4.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="2" spans="1:11" ht="19.5" x14ac:dyDescent="0.3">
       <c r="B2" s="22" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:9" s="23" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" s="23" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="B3" s="24" t="s">
         <v>14</v>
       </c>
@@ -3705,31 +3700,49 @@
         <v>20</v>
       </c>
       <c r="H3" s="26" t="s">
-        <v>21</v>
+        <v>37</v>
+      </c>
+      <c r="I3" s="26" t="s">
+        <v>31</v>
+      </c>
+      <c r="J3" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="K3" s="26" t="s">
+        <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:9" s="23" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" s="23" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="B4" s="24"/>
       <c r="C4" s="25" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D4" s="25" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E4" s="25" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="F4" s="25" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="G4" s="26" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H4" s="25" t="s">
-        <v>23</v>
+        <v>34</v>
+      </c>
+      <c r="I4" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="J4" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="K4" s="25" t="s">
+        <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B5" s="16">
         <v>1</v>
       </c>
@@ -3755,8 +3768,20 @@
         <f>E5^2</f>
         <v>1600</v>
       </c>
+      <c r="I5" s="32">
+        <f>b*C5+b0</f>
+        <v>4.1512125534950073</v>
+      </c>
+      <c r="J5" s="31">
+        <f>D5-I5</f>
+        <v>0.84878744650499272</v>
+      </c>
+      <c r="K5" s="27">
+        <f>J5^2</f>
+        <v>0.72044012934446588</v>
+      </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B6" s="16">
         <v>2</v>
       </c>
@@ -3779,11 +3804,23 @@
         <v>238</v>
       </c>
       <c r="H6" s="27">
-        <f t="shared" ref="H6:H10" si="3">E6^2</f>
+        <f t="shared" ref="H6:I10" si="3">E6^2</f>
         <v>1156</v>
       </c>
+      <c r="I6" s="32">
+        <f>b*C6+b0</f>
+        <v>14.971469329529244</v>
+      </c>
+      <c r="J6" s="31">
+        <f t="shared" ref="J6:J10" si="4">D6-I6</f>
+        <v>2.0285306704707562</v>
+      </c>
+      <c r="K6" s="27">
+        <f t="shared" ref="K6:K10" si="5">J6^2</f>
+        <v>4.1149366810405352</v>
+      </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B7" s="16">
         <v>3</v>
       </c>
@@ -3809,8 +3846,20 @@
         <f t="shared" si="3"/>
         <v>100</v>
       </c>
+      <c r="I7" s="32">
+        <f>b*C7+b0</f>
+        <v>8.5378031383737518</v>
+      </c>
+      <c r="J7" s="31">
+        <f t="shared" si="4"/>
+        <v>2.4621968616262482</v>
+      </c>
+      <c r="K7" s="27">
+        <f t="shared" si="5"/>
+        <v>6.062413385402146</v>
+      </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B8" s="16">
         <v>4</v>
       </c>
@@ -3836,8 +3885,20 @@
         <f t="shared" si="3"/>
         <v>196</v>
       </c>
+      <c r="I8" s="32">
+        <f>b*C8+b0</f>
+        <v>12.047075606276747</v>
+      </c>
+      <c r="J8" s="31">
+        <f t="shared" si="4"/>
+        <v>-4.0470756062767475</v>
+      </c>
+      <c r="K8" s="27">
+        <f t="shared" si="5"/>
+        <v>16.378820962920305</v>
+      </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B9" s="16">
         <v>5</v>
       </c>
@@ -3863,8 +3924,20 @@
         <f t="shared" si="3"/>
         <v>625</v>
       </c>
+      <c r="I9" s="32">
+        <f>b*C9+b0</f>
+        <v>13.655492154065621</v>
+      </c>
+      <c r="J9" s="31">
+        <f t="shared" si="4"/>
+        <v>0.34450784593437866</v>
+      </c>
+      <c r="K9" s="27">
+        <f t="shared" si="5"/>
+        <v>0.11868565591034559</v>
+      </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B10" s="16">
         <v>6</v>
       </c>
@@ -3890,11 +3963,23 @@
         <f t="shared" si="3"/>
         <v>529</v>
       </c>
+      <c r="I10" s="32">
+        <f>b*C10+b0</f>
+        <v>6.6369472182596292</v>
+      </c>
+      <c r="J10" s="31">
+        <f t="shared" si="4"/>
+        <v>-1.6369472182596292</v>
+      </c>
+      <c r="K10" s="27">
+        <f t="shared" si="5"/>
+        <v>2.6795961953679379</v>
+      </c>
     </row>
-    <row r="11" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="5"/>
       <c r="B11" s="19" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C11" s="21">
         <f>AVERAGE(C5:C10)</f>
@@ -3906,7 +3991,7 @@
       </c>
       <c r="E11" s="20"/>
       <c r="F11" s="20" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="G11" s="21">
         <f>SUM(G5:G10)</f>
@@ -3916,8 +4001,16 @@
         <f>SUM(H5:H10)</f>
         <v>4206</v>
       </c>
+      <c r="I11" s="21"/>
+      <c r="J11" s="33" t="s">
+        <v>36</v>
+      </c>
+      <c r="K11" s="33">
+        <f>SUM(K5:K10)</f>
+        <v>30.074893009985736</v>
+      </c>
     </row>
-    <row r="13" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="B13" s="28" t="s">
         <v>8</v>
       </c>
@@ -3927,14 +4020,14 @@
       </c>
       <c r="D13" s="7"/>
       <c r="E13" s="28" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="F13" s="30">
         <f>ymean-C13*xmean</f>
         <v>-0.82025677603423652</v>
       </c>
     </row>
-    <row r="15" spans="1:9" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="B15" s="1"/>
       <c r="C15"/>
       <c r="D15"/>
@@ -3943,14 +4036,16 @@
       <c r="G15"/>
       <c r="H15"/>
       <c r="I15"/>
+      <c r="J15"/>
+      <c r="K15"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B16" s="8"/>
       <c r="E16" s="8"/>
       <c r="F16" s="8"/>
       <c r="G16" s="8"/>
     </row>
-    <row r="18" spans="2:8" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:11" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B18" s="13"/>
       <c r="C18" s="11"/>
       <c r="D18" s="11"/>
@@ -3958,6 +4053,9 @@
       <c r="F18" s="12"/>
       <c r="G18" s="12"/>
       <c r="H18" s="11"/>
+      <c r="I18" s="11"/>
+      <c r="J18" s="11"/>
+      <c r="K18" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
More lectures and practice for regression work
</commit_message>
<xml_diff>
--- a/4_Applied ML with Python/Practice/Lines_Excel_Linear Regression.xlsx
+++ b/4_Applied ML with Python/Practice/Lines_Excel_Linear Regression.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repos\CourseraPlus\4_Applied ML with Python\Practice\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FC9AE8C-11B7-4415-8609-09B6F1668336}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{995899B7-4EAD-4DF0-B805-458A0F3CCA07}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Simple" sheetId="1" r:id="rId1"/>
@@ -162,13 +161,13 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="5">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="0.000000"/>
-    <numFmt numFmtId="165" formatCode="0.0000000"/>
-    <numFmt numFmtId="166" formatCode="_-* #,##0.0000_-;\-* #,##0.0000_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="167" formatCode="_-* #,##0.00000_-;\-* #,##0.00000_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="0.000000"/>
+    <numFmt numFmtId="166" formatCode="0.0000000"/>
+    <numFmt numFmtId="167" formatCode="_-* #,##0.0000_-;\-* #,##0.0000_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="168" formatCode="_-* #,##0.00000_-;\-* #,##0.00000_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="12" x14ac:knownFonts="1">
     <font>
@@ -342,7 +341,7 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -352,35 +351,35 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="165" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="43" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -396,25 +395,25 @@
     <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="4" borderId="0" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="167" fontId="2" fillId="4" borderId="0" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="43" fontId="11" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="2" fillId="4" borderId="0" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="43" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="43" fontId="2" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -424,7 +423,7 @@
   </cellStyles>
   <dxfs count="5">
     <dxf>
-      <numFmt numFmtId="35" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+      <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     </dxf>
     <dxf>
       <font>
@@ -440,10 +439,9 @@
         <sz val="11"/>
         <color rgb="FF002060"/>
         <name val="Arial"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="35" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+      <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     </dxf>
     <dxf>
       <font>
@@ -459,7 +457,6 @@
         <sz val="11"/>
         <color rgb="FF002060"/>
         <name val="Arial"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
     </dxf>
@@ -480,7 +477,6 @@
         <sz val="11"/>
         <color theme="1"/>
         <name val="Arial"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -654,7 +650,7 @@
             <c:numRef>
               <c:f>Simple!$C$4:$C$10</c:f>
               <c:numCache>
-                <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
+                <c:formatCode>_-* #,##0.00_-;\-* #,##0.00_-;_-* "-"??_-;_-@_-</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>1.5</c:v>
@@ -767,7 +763,7 @@
             <c:numRef>
               <c:f>Simple!$D$4:$D$10</c:f>
               <c:numCache>
-                <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
+                <c:formatCode>_-* #,##0.00_-;\-* #,##0.00_-;_-* "-"??_-;_-@_-</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>1.9142857142857099</c:v>
@@ -996,7 +992,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
+        <c:numFmt formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1090,6 +1086,7 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -1097,7 +1094,6 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -1176,6 +1172,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1238,7 +1235,7 @@
             <c:numRef>
               <c:f>'Bill &amp; Tips'!$D$5:$D$10</c:f>
               <c:numCache>
-                <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
+                <c:formatCode>_-* #,##0.00_-;\-* #,##0.00_-;_-* "-"??_-;_-@_-</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>5</c:v>
@@ -1296,7 +1293,7 @@
             <c:numRef>
               <c:f>'Bill &amp; Tips'!$I$5:$I$10</c:f>
               <c:numCache>
-                <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
+                <c:formatCode>_-* #,##0.00_-;\-* #,##0.00_-;_-* "-"??_-;_-@_-</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>4.1512125534950073</c:v>
@@ -1435,6 +1432,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1557,6 +1555,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1585,7 +1584,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
+        <c:numFmt formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1666,6 +1665,7 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -1673,7 +1673,6 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -3027,6 +3026,61 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="95250" y="5086350"/>
+          <a:ext cx="8001000" cy="4505325"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -3080,8 +3134,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{84558B92-8EB9-4E43-8832-DCB27D846770}" name="Table1" displayName="Table1" ref="B3:F11" totalsRowShown="0" headerRowDxfId="4">
-  <autoFilter ref="B3:F11" xr:uid="{84558B92-8EB9-4E43-8832-DCB27D846770}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B3:F11" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="B3:F11">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -3089,13 +3143,13 @@
     <filterColumn colId="4" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{D80E1A59-FE2D-40B7-A59B-EE0E5FE42168}" name="X" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{B098714D-CC10-45C2-8D75-C301525DF26E}" name="y" dataDxfId="2" dataCellStyle="Comma"/>
-    <tableColumn id="6" xr3:uid="{184FA016-1ED8-4EDB-A016-757562BC1DA5}" name="Plot" dataDxfId="1" dataCellStyle="Comma">
+    <tableColumn id="1" name="X" dataDxfId="3"/>
+    <tableColumn id="2" name="y" dataDxfId="2" dataCellStyle="Comma"/>
+    <tableColumn id="6" name="Plot" dataDxfId="1" dataCellStyle="Comma">
       <calculatedColumnFormula>$F$15*Table1[[#This Row],[X]]+$C$15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{334D0BF8-E99F-4951-9277-978C765A67B2}" name="X.y" dataDxfId="0"/>
-    <tableColumn id="4" xr3:uid="{04DCFAC7-F8AC-4F98-A3B8-1467EC661F31}" name="X^2"/>
+    <tableColumn id="3" name="X.y" dataDxfId="0"/>
+    <tableColumn id="4" name="X^2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3397,7 +3451,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B52F56F-293C-43B2-9C80-EEC3C02E9B0E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:F18"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -3652,11 +3706,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB946D3E-1162-4E03-884C-51FAE36A8CB7}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="M38" sqref="M38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -3769,7 +3823,7 @@
         <v>1600</v>
       </c>
       <c r="I5" s="32">
-        <f>b*C5+b0</f>
+        <f t="shared" ref="I5:I10" si="2">b*C5+b0</f>
         <v>4.1512125534950073</v>
       </c>
       <c r="J5" s="31">
@@ -3800,23 +3854,23 @@
         <v>7</v>
       </c>
       <c r="G6" s="18">
-        <f t="shared" ref="G6:G10" si="2">E6*F6</f>
+        <f t="shared" ref="G6:G10" si="3">E6*F6</f>
         <v>238</v>
       </c>
       <c r="H6" s="27">
-        <f t="shared" ref="H6:I10" si="3">E6^2</f>
+        <f t="shared" ref="H6:H10" si="4">E6^2</f>
         <v>1156</v>
       </c>
       <c r="I6" s="32">
-        <f>b*C6+b0</f>
+        <f t="shared" si="2"/>
         <v>14.971469329529244</v>
       </c>
       <c r="J6" s="31">
-        <f t="shared" ref="J6:J10" si="4">D6-I6</f>
+        <f t="shared" ref="J6:J10" si="5">D6-I6</f>
         <v>2.0285306704707562</v>
       </c>
       <c r="K6" s="27">
-        <f t="shared" ref="K6:K10" si="5">J6^2</f>
+        <f t="shared" ref="K6:K10" si="6">J6^2</f>
         <v>4.1149366810405352</v>
       </c>
     </row>
@@ -3839,23 +3893,23 @@
         <v>1</v>
       </c>
       <c r="G7" s="18">
+        <f t="shared" si="3"/>
+        <v>-10</v>
+      </c>
+      <c r="H7" s="27">
+        <f t="shared" si="4"/>
+        <v>100</v>
+      </c>
+      <c r="I7" s="32">
         <f t="shared" si="2"/>
-        <v>-10</v>
-      </c>
-      <c r="H7" s="27">
-        <f t="shared" si="3"/>
-        <v>100</v>
-      </c>
-      <c r="I7" s="32">
-        <f>b*C7+b0</f>
         <v>8.5378031383737518</v>
       </c>
       <c r="J7" s="31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2.4621968616262482</v>
       </c>
       <c r="K7" s="27">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>6.062413385402146</v>
       </c>
     </row>
@@ -3878,23 +3932,23 @@
         <v>-2</v>
       </c>
       <c r="G8" s="18">
+        <f t="shared" si="3"/>
+        <v>-28</v>
+      </c>
+      <c r="H8" s="27">
+        <f t="shared" si="4"/>
+        <v>196</v>
+      </c>
+      <c r="I8" s="32">
         <f t="shared" si="2"/>
-        <v>-28</v>
-      </c>
-      <c r="H8" s="27">
-        <f t="shared" si="3"/>
-        <v>196</v>
-      </c>
-      <c r="I8" s="32">
-        <f>b*C8+b0</f>
         <v>12.047075606276747</v>
       </c>
       <c r="J8" s="31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-4.0470756062767475</v>
       </c>
       <c r="K8" s="27">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>16.378820962920305</v>
       </c>
     </row>
@@ -3917,23 +3971,23 @@
         <v>4</v>
       </c>
       <c r="G9" s="18">
+        <f t="shared" si="3"/>
+        <v>100</v>
+      </c>
+      <c r="H9" s="27">
+        <f t="shared" si="4"/>
+        <v>625</v>
+      </c>
+      <c r="I9" s="32">
         <f t="shared" si="2"/>
-        <v>100</v>
-      </c>
-      <c r="H9" s="27">
-        <f t="shared" si="3"/>
-        <v>625</v>
-      </c>
-      <c r="I9" s="32">
-        <f>b*C9+b0</f>
         <v>13.655492154065621</v>
       </c>
       <c r="J9" s="31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.34450784593437866</v>
       </c>
       <c r="K9" s="27">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.11868565591034559</v>
       </c>
     </row>
@@ -3956,23 +4010,23 @@
         <v>-5</v>
       </c>
       <c r="G10" s="18">
+        <f t="shared" si="3"/>
+        <v>115</v>
+      </c>
+      <c r="H10" s="27">
+        <f t="shared" si="4"/>
+        <v>529</v>
+      </c>
+      <c r="I10" s="32">
         <f t="shared" si="2"/>
-        <v>115</v>
-      </c>
-      <c r="H10" s="27">
-        <f t="shared" si="3"/>
-        <v>529</v>
-      </c>
-      <c r="I10" s="32">
-        <f>b*C10+b0</f>
         <v>6.6369472182596292</v>
       </c>
       <c r="J10" s="31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-1.6369472182596292</v>
       </c>
       <c r="K10" s="27">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>2.6795961953679379</v>
       </c>
     </row>
@@ -4065,7 +4119,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{444B31FE-9D94-4105-9694-D16CEE94268F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>